<commit_message>
Deploying to gh-pages from  @ 0c7d8622007b10b5afb2d3f3c1c6b1d230dd6159 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-4-4.xlsx
+++ b/assets/excel/2021_1-4-4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{984D32AE-8D77-4CED-A4A5-017C7775A19C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD66855-BEB0-40AE-9112-1F0398886D74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{F38A3A7E-7467-443D-941C-8491F7F21352}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -82,6 +82,18 @@
   <si>
     <t>Quelle: Wanderungsstatistik</t>
   </si>
+  <si>
+    <t>Niedersächsisches Ministerium für Soziales, Gesundheit und Gleichstellung (Hrsg.),</t>
+  </si>
+  <si>
+    <t>© Landesamt für Statistik Niedersachsen, Hannover 2021,                                                                          </t>
+  </si>
+  <si>
+    <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangabe gestattet.</t>
+  </si>
+  <si>
+    <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +105,7 @@
     <numFmt numFmtId="166" formatCode="###\ ###\ ###"/>
     <numFmt numFmtId="167" formatCode="\+##\ ###;\-##\ ###"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +124,20 @@
     <font>
       <sz val="6"/>
       <color theme="1"/>
+      <name val="NDSFrutiger 45 Light"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="6"/>
+      <color theme="10"/>
       <name val="NDSFrutiger 45 Light"/>
     </font>
   </fonts>
@@ -195,10 +221,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -210,18 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -275,8 +290,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,7 +620,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CC28A7-E2AE-4694-96A0-3192D5CBA853}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:L59"/>
+  <dimension ref="B1:L64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:B8"/>
@@ -664,1666 +694,1666 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="11"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="27">
+      <c r="B9" s="23">
         <v>1</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="23">
         <v>3</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="24">
         <v>4</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="23">
         <v>5</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="24">
         <v>6</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="23">
         <v>7</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="24">
         <v>8</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="23">
         <v>9</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="24">
         <v>10</v>
       </c>
-      <c r="L9" s="11"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>2020</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <v>113276</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="13">
         <v>4805</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="13">
         <v>8395</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="13">
         <v>6749</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="13">
         <v>61378</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="13">
         <v>29966</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="13">
         <v>1732</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="13">
         <v>251</v>
       </c>
-      <c r="L10" s="11"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="8">
         <v>2020</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <v>86127</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="13">
         <v>2586</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="13">
         <v>3411</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="13">
         <v>3561</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="13">
         <v>48443</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="13">
         <v>25863</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="13">
         <v>1878</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="13">
         <v>385</v>
       </c>
-      <c r="L11" s="11"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
+      <c r="B12" s="8">
         <v>2020</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <v>27149</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="11">
         <v>2219</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="11">
         <v>4984</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="11">
         <v>3188</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="11">
         <v>12935</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="11">
         <v>4103</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="11">
         <v>-146</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="11">
         <v>-134</v>
       </c>
-      <c r="L12" s="11"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="B13" s="9">
         <v>2019</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="10">
         <v>151149</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="10">
         <v>6390</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="10">
         <v>11833</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="10">
         <v>9810</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="10">
         <v>82028</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="10">
         <v>38665</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="10">
         <v>2116</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="10">
         <v>307</v>
       </c>
-      <c r="L13" s="11"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="13">
+      <c r="B14" s="9">
         <v>2019</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="10">
         <v>112933</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="10">
         <v>3071</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="10">
         <v>4401</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="10">
         <v>5035</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="10">
         <v>64223</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="10">
         <v>33180</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="10">
         <v>2493</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="10">
         <v>530</v>
       </c>
-      <c r="L14" s="11"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
+      <c r="B15" s="9">
         <v>2019</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="11">
         <v>38216</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="11">
         <v>3319</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="11">
         <v>7432</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="11">
         <v>4775</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="11">
         <v>17805</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="11">
         <v>5485</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="11">
         <v>-377</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="11">
         <v>-223</v>
       </c>
-      <c r="L15" s="11"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="13">
+      <c r="B16" s="9">
         <v>2018</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="13">
         <v>154372</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="13">
         <v>6364</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="13">
         <v>11656</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="13">
         <v>10235</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="13">
         <v>84313</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="13">
         <v>39425</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="13">
         <v>2092</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="13">
         <v>287</v>
       </c>
-      <c r="L16" s="18"/>
+      <c r="L16" s="14"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="13">
+      <c r="B17" s="9">
         <v>2018</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="13">
         <v>109363</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="13">
         <v>3219</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="13">
         <v>4670</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="13">
         <v>5204</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="13">
         <v>62735</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="13">
         <v>30996</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="13">
         <v>2139</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="13">
         <v>400</v>
       </c>
-      <c r="L17" s="18"/>
+      <c r="L17" s="14"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="13">
+      <c r="B18" s="9">
         <v>2018</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <v>45009</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="15">
         <v>3145</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <v>6986</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <v>5031</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="15">
         <v>21578</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="15">
         <v>8429</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="15">
         <v>-47</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="15">
         <v>-113</v>
       </c>
-      <c r="L18" s="20"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="13">
+      <c r="B19" s="9">
         <v>2017</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="13">
         <v>145901</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="13">
         <v>6722</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="13">
         <v>12249</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="13">
         <v>10053</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="13">
         <v>79251</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="13">
         <v>35487</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="13">
         <v>1878</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K19" s="13">
         <v>261</v>
       </c>
-      <c r="L19" s="11"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="13">
+      <c r="B20" s="9">
         <v>2017</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="13">
         <v>107296</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="13">
         <v>3381</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="13">
         <v>4901</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="13">
         <v>5170</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="13">
         <v>62067</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="13">
         <v>29342</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="13">
         <v>1998</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="13">
         <v>437</v>
       </c>
-      <c r="L20" s="18"/>
+      <c r="L20" s="14"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="13">
+      <c r="B21" s="9">
         <v>2017</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="15">
         <v>38605</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="15">
         <v>3341</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="15">
         <v>7348</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="15">
         <v>4883</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="15">
         <v>17184</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="15">
         <v>6145</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J21" s="15">
         <v>-120</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="15">
         <v>-176</v>
       </c>
-      <c r="L21" s="20"/>
+      <c r="L21" s="16"/>
     </row>
     <row r="22" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="21">
+      <c r="B22" s="17">
         <v>2016</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="18">
         <v>175201</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="19">
         <v>10213</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="19">
         <v>18470</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="19">
         <v>15669</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="19">
         <v>91735</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="19">
         <v>36957</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="19">
         <v>1884</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="19">
         <v>273</v>
       </c>
-      <c r="L22" s="11"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="21">
+      <c r="B23" s="17">
         <v>2016</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="18">
         <v>137021</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="19">
         <v>5257</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="19">
         <v>8355</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="19">
         <v>7105</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="19">
         <v>79448</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="19">
         <v>34215</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="19">
         <v>2172</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="19">
         <v>469</v>
       </c>
-      <c r="L23" s="11"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="21">
+      <c r="B24" s="17">
         <v>2016</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="20">
         <v>38180</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="20">
         <v>4956</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24" s="20">
         <v>10115</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="20">
         <v>8564</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="20">
         <v>12287</v>
       </c>
-      <c r="I24" s="24">
+      <c r="I24" s="20">
         <v>2742</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="20">
         <v>-288</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="20">
         <v>-196</v>
       </c>
-      <c r="L24" s="11"/>
+      <c r="L24" s="7"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="21">
+      <c r="B25" s="17">
         <v>2015</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="21">
         <v>206650</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="21">
         <v>12281</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="21">
         <v>21455</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="21">
         <v>17587</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="21">
         <v>112526</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="21">
         <v>40575</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25" s="21">
         <v>1969</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="21">
         <v>257</v>
       </c>
-      <c r="L25" s="11"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="21">
+      <c r="B26" s="17">
         <v>2015</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="21">
         <v>87051</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="21">
         <v>2517</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="21">
         <v>4183</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="21">
         <v>3913</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="21">
         <v>50914</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="21">
         <v>23775</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="21">
         <v>1513</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="21">
         <v>236</v>
       </c>
-      <c r="L26" s="11"/>
+      <c r="L26" s="7"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="21">
+      <c r="B27" s="17">
         <v>2015</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="20">
         <v>119599</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="20">
         <v>9764</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="20">
         <v>17272</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="20">
         <v>13674</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="20">
         <v>61612</v>
       </c>
-      <c r="I27" s="24">
+      <c r="I27" s="20">
         <v>16800</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J27" s="20">
         <v>456</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="20">
         <v>21</v>
       </c>
-      <c r="L27" s="11"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="21">
+      <c r="B28" s="17">
         <v>2014</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="21">
         <v>139181</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="21">
         <v>6504</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="21">
         <v>11076</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="21">
         <v>8697</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="21">
         <v>77407</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="21">
         <v>33483</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="21">
         <v>1774</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="21">
         <v>240</v>
       </c>
-      <c r="L28" s="11"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="21">
+      <c r="B29" s="17">
         <v>2014</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="21">
         <v>85138</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="21">
         <v>2001</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="21">
         <v>3261</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="21">
         <v>3274</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="21">
         <v>49600</v>
       </c>
-      <c r="I29" s="25">
+      <c r="I29" s="21">
         <v>24998</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="21">
         <v>1738</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="21">
         <v>266</v>
       </c>
-      <c r="L29" s="11"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="21">
+      <c r="B30" s="17">
         <v>2014</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="20">
         <v>54043</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="20">
         <v>4503</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="20">
         <v>7815</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="20">
         <v>5423</v>
       </c>
-      <c r="H30" s="24">
+      <c r="H30" s="20">
         <v>27807</v>
       </c>
-      <c r="I30" s="24">
+      <c r="I30" s="20">
         <v>8485</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="20">
         <v>36</v>
       </c>
-      <c r="K30" s="24">
+      <c r="K30" s="20">
         <v>-245</v>
       </c>
-      <c r="L30" s="11"/>
+      <c r="L30" s="7"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="21">
+      <c r="B31" s="17">
         <v>2013</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="21">
         <v>110921</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="21">
         <v>4625</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="21">
         <v>6842</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="21">
         <v>6273</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="21">
         <v>63511</v>
       </c>
-      <c r="I31" s="25">
+      <c r="I31" s="21">
         <v>28096</v>
       </c>
-      <c r="J31" s="25">
+      <c r="J31" s="21">
         <v>1407</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="21">
         <v>167</v>
       </c>
-      <c r="L31" s="11"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="21">
+      <c r="B32" s="17">
         <v>2013</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="21">
         <v>75986</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="21">
         <v>1756</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="21">
         <v>2656</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="21">
         <v>2853</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="21">
         <v>44043</v>
       </c>
-      <c r="I32" s="25">
+      <c r="I32" s="21">
         <v>23110</v>
       </c>
-      <c r="J32" s="25">
+      <c r="J32" s="21">
         <v>1370</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="21">
         <v>198</v>
       </c>
-      <c r="L32" s="11"/>
+      <c r="L32" s="7"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="21">
+      <c r="B33" s="17">
         <v>2013</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="20">
         <v>34935</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E33" s="20">
         <v>2869</v>
       </c>
-      <c r="F33" s="24">
+      <c r="F33" s="20">
         <v>4186</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="20">
         <v>3420</v>
       </c>
-      <c r="H33" s="24">
+      <c r="H33" s="20">
         <v>19468</v>
       </c>
-      <c r="I33" s="24">
+      <c r="I33" s="20">
         <v>4986</v>
       </c>
-      <c r="J33" s="24">
+      <c r="J33" s="20">
         <v>37</v>
       </c>
-      <c r="K33" s="24">
+      <c r="K33" s="20">
         <v>-31</v>
       </c>
-      <c r="L33" s="11"/>
+      <c r="L33" s="7"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="21">
+      <c r="B34" s="17">
         <v>2012</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="21">
         <v>99001</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="21">
         <v>3494</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="21">
         <v>5151</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="21">
         <v>5208</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="21">
         <v>57727</v>
       </c>
-      <c r="I34" s="25">
+      <c r="I34" s="21">
         <v>26129</v>
       </c>
-      <c r="J34" s="25">
+      <c r="J34" s="21">
         <v>1118</v>
       </c>
-      <c r="K34" s="25">
+      <c r="K34" s="21">
         <v>174</v>
       </c>
-      <c r="L34" s="11"/>
+      <c r="L34" s="7"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="21">
+      <c r="B35" s="17">
         <v>2012</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="21">
         <v>71481</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="21">
         <v>1545</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="21">
         <v>2609</v>
       </c>
-      <c r="G35" s="25">
+      <c r="G35" s="21">
         <v>2732</v>
       </c>
-      <c r="H35" s="25">
+      <c r="H35" s="21">
         <v>41110</v>
       </c>
-      <c r="I35" s="25">
+      <c r="I35" s="21">
         <v>21870</v>
       </c>
-      <c r="J35" s="25">
+      <c r="J35" s="21">
         <v>1393</v>
       </c>
-      <c r="K35" s="25">
+      <c r="K35" s="21">
         <v>222</v>
       </c>
-      <c r="L35" s="11"/>
+      <c r="L35" s="7"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="21">
+      <c r="B36" s="17">
         <v>2012</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="20">
         <v>27520</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="20">
         <v>1949</v>
       </c>
-      <c r="F36" s="24">
+      <c r="F36" s="20">
         <v>2542</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="20">
         <v>2476</v>
       </c>
-      <c r="H36" s="24">
+      <c r="H36" s="20">
         <v>16617</v>
       </c>
-      <c r="I36" s="24">
+      <c r="I36" s="20">
         <v>4259</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="20">
         <v>-275</v>
       </c>
-      <c r="K36" s="24">
+      <c r="K36" s="20">
         <v>-48</v>
       </c>
-      <c r="L36" s="11"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="21">
+      <c r="B37" s="17">
         <v>2011</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="25">
+      <c r="D37" s="21">
         <v>91507</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="21">
         <v>2888</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="21">
         <v>4263</v>
       </c>
-      <c r="G37" s="25">
+      <c r="G37" s="21">
         <v>5019</v>
       </c>
-      <c r="H37" s="25">
+      <c r="H37" s="21">
         <v>52602</v>
       </c>
-      <c r="I37" s="25">
+      <c r="I37" s="21">
         <v>25444</v>
       </c>
-      <c r="J37" s="25">
+      <c r="J37" s="21">
         <v>1108</v>
       </c>
-      <c r="K37" s="25">
+      <c r="K37" s="21">
         <v>183</v>
       </c>
-      <c r="L37" s="11"/>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="21">
+      <c r="B38" s="17">
         <v>2011</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="25">
+      <c r="D38" s="21">
         <v>67837</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="21">
         <v>1515</v>
       </c>
-      <c r="F38" s="25">
+      <c r="F38" s="21">
         <v>2568</v>
       </c>
-      <c r="G38" s="25">
+      <c r="G38" s="21">
         <v>2876</v>
       </c>
-      <c r="H38" s="25">
+      <c r="H38" s="21">
         <v>38547</v>
       </c>
-      <c r="I38" s="25">
+      <c r="I38" s="21">
         <v>20815</v>
       </c>
-      <c r="J38" s="25">
+      <c r="J38" s="21">
         <v>1343</v>
       </c>
-      <c r="K38" s="25">
+      <c r="K38" s="21">
         <v>173</v>
       </c>
-      <c r="L38" s="11"/>
+      <c r="L38" s="7"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="21">
+      <c r="B39" s="17">
         <v>2011</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="20">
         <v>23670</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="20">
         <v>1373</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="20">
         <v>1695</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="20">
         <v>2143</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="20">
         <v>14055</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="20">
         <v>4629</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="20">
         <v>-235</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="20">
         <v>10</v>
       </c>
-      <c r="L39" s="11"/>
+      <c r="L39" s="7"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="21">
+      <c r="B40" s="17">
         <v>2010</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="25">
+      <c r="D40" s="21">
         <v>76783</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="21">
         <v>2485</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="21">
         <v>3668</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="21">
         <v>4389</v>
       </c>
-      <c r="H40" s="25">
+      <c r="H40" s="21">
         <v>44374</v>
       </c>
-      <c r="I40" s="25">
+      <c r="I40" s="21">
         <v>20561</v>
       </c>
-      <c r="J40" s="25">
+      <c r="J40" s="21">
         <v>1148</v>
       </c>
-      <c r="K40" s="25">
+      <c r="K40" s="21">
         <v>158</v>
       </c>
-      <c r="L40" s="11"/>
+      <c r="L40" s="7"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="21">
+      <c r="B41" s="17">
         <v>2010</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="21">
         <v>62325</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="21">
         <v>1261</v>
       </c>
-      <c r="F41" s="25">
+      <c r="F41" s="21">
         <v>2302</v>
       </c>
-      <c r="G41" s="25">
+      <c r="G41" s="21">
         <v>2690</v>
       </c>
-      <c r="H41" s="25">
+      <c r="H41" s="21">
         <v>36043</v>
       </c>
-      <c r="I41" s="25">
+      <c r="I41" s="21">
         <v>18419</v>
       </c>
-      <c r="J41" s="25">
+      <c r="J41" s="21">
         <v>1379</v>
       </c>
-      <c r="K41" s="25">
+      <c r="K41" s="21">
         <v>231</v>
       </c>
-      <c r="L41" s="11"/>
+      <c r="L41" s="7"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="21">
+      <c r="B42" s="17">
         <v>2010</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="20">
         <v>14458</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="20">
         <v>1224</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="20">
         <v>1366</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="20">
         <v>1699</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H42" s="20">
         <v>8331</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I42" s="20">
         <v>2142</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="20">
         <v>-231</v>
       </c>
-      <c r="K42" s="24">
+      <c r="K42" s="20">
         <v>-73</v>
       </c>
-      <c r="L42" s="11"/>
+      <c r="L42" s="7"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="21">
+      <c r="B43" s="17">
         <v>2009</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="21">
         <v>73925</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="21">
         <v>2383</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="21">
         <v>3623</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="21">
         <v>4434</v>
       </c>
-      <c r="H43" s="25">
+      <c r="H43" s="21">
         <v>41755</v>
       </c>
-      <c r="I43" s="25">
+      <c r="I43" s="21">
         <v>20294</v>
       </c>
-      <c r="J43" s="25">
+      <c r="J43" s="21">
         <v>1259</v>
       </c>
-      <c r="K43" s="25">
+      <c r="K43" s="21">
         <v>177</v>
       </c>
-      <c r="L43" s="11"/>
+      <c r="L43" s="7"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="21">
+      <c r="B44" s="17">
         <v>2009</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="25">
+      <c r="D44" s="21">
         <v>66282</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="21">
         <v>1310</v>
       </c>
-      <c r="F44" s="25">
+      <c r="F44" s="21">
         <v>2520</v>
       </c>
-      <c r="G44" s="25">
+      <c r="G44" s="21">
         <v>2938</v>
       </c>
-      <c r="H44" s="25">
+      <c r="H44" s="21">
         <v>37350</v>
       </c>
-      <c r="I44" s="25">
+      <c r="I44" s="21">
         <v>20223</v>
       </c>
-      <c r="J44" s="25">
+      <c r="J44" s="21">
         <v>1683</v>
       </c>
-      <c r="K44" s="25">
+      <c r="K44" s="21">
         <v>258</v>
       </c>
-      <c r="L44" s="11"/>
+      <c r="L44" s="7"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="21">
+      <c r="B45" s="17">
         <v>2009</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="20">
         <v>7643</v>
       </c>
-      <c r="E45" s="24">
+      <c r="E45" s="20">
         <v>1073</v>
       </c>
-      <c r="F45" s="24">
+      <c r="F45" s="20">
         <v>1103</v>
       </c>
-      <c r="G45" s="24">
+      <c r="G45" s="20">
         <v>1496</v>
       </c>
-      <c r="H45" s="24">
+      <c r="H45" s="20">
         <v>4405</v>
       </c>
-      <c r="I45" s="24">
+      <c r="I45" s="20">
         <v>71</v>
       </c>
-      <c r="J45" s="24">
+      <c r="J45" s="20">
         <v>-424</v>
       </c>
-      <c r="K45" s="24">
+      <c r="K45" s="20">
         <v>-81</v>
       </c>
-      <c r="L45" s="11"/>
+      <c r="L45" s="7"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="21">
+      <c r="B46" s="17">
         <v>2008</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="25">
+      <c r="D46" s="21">
         <v>69064</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="21">
         <v>2036</v>
       </c>
-      <c r="F46" s="25">
+      <c r="F46" s="21">
         <v>3061</v>
       </c>
-      <c r="G46" s="25">
+      <c r="G46" s="21">
         <v>4102</v>
       </c>
-      <c r="H46" s="25">
+      <c r="H46" s="21">
         <v>39642</v>
       </c>
-      <c r="I46" s="25">
+      <c r="I46" s="21">
         <v>18730</v>
       </c>
-      <c r="J46" s="25">
+      <c r="J46" s="21">
         <v>1317</v>
       </c>
-      <c r="K46" s="25">
+      <c r="K46" s="21">
         <v>176</v>
       </c>
-      <c r="L46" s="11"/>
+      <c r="L46" s="7"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="21">
+      <c r="B47" s="17">
         <v>2008</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="25">
+      <c r="D47" s="21">
         <v>68114</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="21">
         <v>1453</v>
       </c>
-      <c r="F47" s="25">
+      <c r="F47" s="21">
         <v>2854</v>
       </c>
-      <c r="G47" s="25">
+      <c r="G47" s="21">
         <v>3093</v>
       </c>
-      <c r="H47" s="25">
+      <c r="H47" s="21">
         <v>39104</v>
       </c>
-      <c r="I47" s="25">
+      <c r="I47" s="21">
         <v>19736</v>
       </c>
-      <c r="J47" s="25">
+      <c r="J47" s="21">
         <v>1628</v>
       </c>
-      <c r="K47" s="25">
+      <c r="K47" s="21">
         <v>246</v>
       </c>
-      <c r="L47" s="11"/>
+      <c r="L47" s="7"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="21">
+      <c r="B48" s="17">
         <v>2008</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48" s="20">
         <v>950</v>
       </c>
-      <c r="E48" s="24">
+      <c r="E48" s="20">
         <v>583</v>
       </c>
-      <c r="F48" s="24">
+      <c r="F48" s="20">
         <v>207</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G48" s="20">
         <v>1009</v>
       </c>
-      <c r="H48" s="24">
+      <c r="H48" s="20">
         <v>538</v>
       </c>
-      <c r="I48" s="24">
+      <c r="I48" s="20">
         <v>-1006</v>
       </c>
-      <c r="J48" s="24">
+      <c r="J48" s="20">
         <v>-311</v>
       </c>
-      <c r="K48" s="24">
+      <c r="K48" s="20">
         <v>-70</v>
       </c>
-      <c r="L48" s="11"/>
+      <c r="L48" s="7"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="21">
+      <c r="B49" s="17">
         <v>2007</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="25">
+      <c r="D49" s="21">
         <v>70754</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="21">
         <v>2033</v>
       </c>
-      <c r="F49" s="25">
+      <c r="F49" s="21">
         <v>3340</v>
       </c>
-      <c r="G49" s="25">
+      <c r="G49" s="21">
         <v>4070</v>
       </c>
-      <c r="H49" s="25">
+      <c r="H49" s="21">
         <v>41051</v>
       </c>
-      <c r="I49" s="25">
+      <c r="I49" s="21">
         <v>18476</v>
       </c>
-      <c r="J49" s="25">
+      <c r="J49" s="21">
         <v>1610</v>
       </c>
-      <c r="K49" s="25">
+      <c r="K49" s="21">
         <v>174</v>
       </c>
-      <c r="L49" s="11"/>
+      <c r="L49" s="7"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="21">
+      <c r="B50" s="17">
         <v>2007</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="25">
+      <c r="D50" s="21">
         <v>59027</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="21">
         <v>1280</v>
       </c>
-      <c r="F50" s="25">
+      <c r="F50" s="21">
         <v>2538</v>
       </c>
-      <c r="G50" s="25">
+      <c r="G50" s="21">
         <v>2722</v>
       </c>
-      <c r="H50" s="25">
+      <c r="H50" s="21">
         <v>35363</v>
       </c>
-      <c r="I50" s="25">
+      <c r="I50" s="21">
         <v>15776</v>
       </c>
-      <c r="J50" s="25">
+      <c r="J50" s="21">
         <v>1179</v>
       </c>
-      <c r="K50" s="25">
+      <c r="K50" s="21">
         <v>169</v>
       </c>
-      <c r="L50" s="11"/>
+      <c r="L50" s="7"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" s="21">
+      <c r="B51" s="17">
         <v>2007</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51" s="20">
         <v>11727</v>
       </c>
-      <c r="E51" s="24">
+      <c r="E51" s="20">
         <v>753</v>
       </c>
-      <c r="F51" s="24">
+      <c r="F51" s="20">
         <v>802</v>
       </c>
-      <c r="G51" s="24">
+      <c r="G51" s="20">
         <v>1348</v>
       </c>
-      <c r="H51" s="24">
+      <c r="H51" s="20">
         <v>5688</v>
       </c>
-      <c r="I51" s="24">
+      <c r="I51" s="20">
         <v>2700</v>
       </c>
-      <c r="J51" s="24">
+      <c r="J51" s="20">
         <v>431</v>
       </c>
-      <c r="K51" s="24">
+      <c r="K51" s="20">
         <v>5</v>
       </c>
-      <c r="L51" s="11"/>
+      <c r="L51" s="7"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="21">
+      <c r="B52" s="17">
         <v>2006</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D52" s="21">
         <v>69486</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="21">
         <v>2133</v>
       </c>
-      <c r="F52" s="25">
+      <c r="F52" s="21">
         <v>3498</v>
       </c>
-      <c r="G52" s="25">
+      <c r="G52" s="21">
         <v>3909</v>
       </c>
-      <c r="H52" s="25">
+      <c r="H52" s="21">
         <v>40505</v>
       </c>
-      <c r="I52" s="25">
+      <c r="I52" s="21">
         <v>17646</v>
       </c>
-      <c r="J52" s="25">
+      <c r="J52" s="21">
         <v>1633</v>
       </c>
-      <c r="K52" s="25">
+      <c r="K52" s="21">
         <v>162</v>
       </c>
-      <c r="L52" s="11"/>
+      <c r="L52" s="7"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="21">
+      <c r="B53" s="17">
         <v>2006</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="25">
+      <c r="D53" s="21">
         <v>56337</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="21">
         <v>1240</v>
       </c>
-      <c r="F53" s="25">
+      <c r="F53" s="21">
         <v>2603</v>
       </c>
-      <c r="G53" s="25">
+      <c r="G53" s="21">
         <v>2392</v>
       </c>
-      <c r="H53" s="25">
+      <c r="H53" s="21">
         <v>34098</v>
       </c>
-      <c r="I53" s="25">
+      <c r="I53" s="21">
         <v>14590</v>
       </c>
-      <c r="J53" s="25">
+      <c r="J53" s="21">
         <v>1256</v>
       </c>
-      <c r="K53" s="25">
+      <c r="K53" s="21">
         <v>158</v>
       </c>
-      <c r="L53" s="11"/>
+      <c r="L53" s="7"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="21">
+      <c r="B54" s="17">
         <v>2006</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="24">
+      <c r="D54" s="20">
         <v>13149</v>
       </c>
-      <c r="E54" s="24">
+      <c r="E54" s="20">
         <v>893</v>
       </c>
-      <c r="F54" s="24">
+      <c r="F54" s="20">
         <v>895</v>
       </c>
-      <c r="G54" s="24">
+      <c r="G54" s="20">
         <v>1517</v>
       </c>
-      <c r="H54" s="24">
+      <c r="H54" s="20">
         <v>6407</v>
       </c>
-      <c r="I54" s="24">
+      <c r="I54" s="20">
         <v>3056</v>
       </c>
-      <c r="J54" s="24">
+      <c r="J54" s="20">
         <v>377</v>
       </c>
-      <c r="K54" s="24">
+      <c r="K54" s="20">
         <v>4</v>
       </c>
-      <c r="L54" s="11"/>
+      <c r="L54" s="7"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="21">
+      <c r="B55" s="17">
         <v>2005</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="25">
+      <c r="D55" s="21">
         <v>95893</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="21">
         <v>3723</v>
       </c>
-      <c r="F55" s="25">
+      <c r="F55" s="21">
         <v>7615</v>
       </c>
-      <c r="G55" s="25">
+      <c r="G55" s="21">
         <v>6459</v>
       </c>
-      <c r="H55" s="25">
+      <c r="H55" s="21">
         <v>50935</v>
       </c>
-      <c r="I55" s="25">
+      <c r="I55" s="21">
         <v>23652</v>
       </c>
-      <c r="J55" s="25">
+      <c r="J55" s="21">
         <v>3208</v>
       </c>
-      <c r="K55" s="25">
+      <c r="K55" s="21">
         <v>301</v>
       </c>
       <c r="L55" s="1"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="21">
+      <c r="B56" s="17">
         <v>2005</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D56" s="21">
         <v>55376</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="21">
         <v>1364</v>
       </c>
-      <c r="F56" s="25">
+      <c r="F56" s="21">
         <v>2799</v>
       </c>
-      <c r="G56" s="25">
+      <c r="G56" s="21">
         <v>2352</v>
       </c>
-      <c r="H56" s="25">
+      <c r="H56" s="21">
         <v>33801</v>
       </c>
-      <c r="I56" s="25">
+      <c r="I56" s="21">
         <v>13785</v>
       </c>
-      <c r="J56" s="25">
+      <c r="J56" s="21">
         <v>1125</v>
       </c>
-      <c r="K56" s="25">
+      <c r="K56" s="21">
         <v>150</v>
       </c>
       <c r="L56" s="1"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="21">
+      <c r="B57" s="17">
         <v>2005</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="20">
         <v>40517</v>
       </c>
-      <c r="E57" s="24">
+      <c r="E57" s="20">
         <v>2359</v>
       </c>
-      <c r="F57" s="24">
+      <c r="F57" s="20">
         <v>4816</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G57" s="20">
         <v>4107</v>
       </c>
-      <c r="H57" s="24">
+      <c r="H57" s="20">
         <v>17134</v>
       </c>
-      <c r="I57" s="24">
+      <c r="I57" s="20">
         <v>9867</v>
       </c>
-      <c r="J57" s="24">
+      <c r="J57" s="20">
         <v>2083</v>
       </c>
-      <c r="K57" s="24">
+      <c r="K57" s="20">
         <v>151</v>
       </c>
       <c r="L57" s="1"/>
@@ -2342,7 +2372,7 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C59" s="1"/>
@@ -2356,6 +2386,30 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
+    <row r="61" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="29"/>
+    </row>
+    <row r="62" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="29"/>
+    </row>
+    <row r="63" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="29"/>
+    </row>
+    <row r="64" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" s="29"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B7:B8"/>
@@ -2363,6 +2417,10 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:K7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B64" r:id="rId1" xr:uid="{41ECC942-66F5-4833-959D-CD30B9EC686D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>